<commit_message>
Update import feature from excel Stock Entry : 'Import Material Issue Stock Entry' , 'Import Material Issue Stock Entry' Item : 'Create Item Variants From Excel'
</commit_message>
<xml_diff>
--- a/customize_erpnext/api/bulk_update_scripts/create_item_variants_improved_template.xlsx
+++ b/customize_erpnext/api/bulk_update_scripts/create_item_variants_improved_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://torayqn-my.sharepoint.com/personal/son_nt_tiqn_com_vn/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\son.nt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0866922A-A23E-46FC-A129-D5B4950467D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DC80DD-B516-41FD-9D53-6B835F1E0AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA10BF28-4140-4CA8-83EC-BB6A0348ECDA}"/>
   </bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="184">
   <si>
     <t>26Ss(SMS)</t>
   </si>
@@ -619,9 +619,6 @@
     <t>FXR1132DWR-BS-NF</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Attribute Info - Value</t>
   </si>
   <si>
@@ -641,6 +638,18 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Cột xanh : bắt buộc</t>
+  </si>
+  <si>
+    <t>Cột xám : tùy chọn</t>
+  </si>
+  <si>
+    <t>Item template tương ứng với Item Name (Art No) phải tồn tại trên hệ thống</t>
+  </si>
+  <si>
+    <t>Các thuộc tính color, size, brand, season, info phải tồn tại trên hệ thống</t>
   </si>
 </sst>
 </file>
@@ -663,14 +672,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -683,8 +684,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -694,6 +702,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,31 +737,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{F2FDB0A5-888D-4358-8359-0627D3E749F6}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -996,8 +1071,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{6AF28CCF-2739-41B5-B0E8-CB47BAC39E5B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="69" unboundColumnsRight="1">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="69">
+    <queryTableFields count="7">
       <queryTableField id="58" name="Index" tableColumnId="12"/>
       <queryTableField id="2" name="Item Name" tableColumnId="2"/>
       <queryTableField id="5" name="Attribute Color - Value" tableColumnId="5"/>
@@ -1005,7 +1080,6 @@
       <queryTableField id="9" name="Attribute Brand - Value" tableColumnId="9"/>
       <queryTableField id="11" name="Attribute Season - Value" tableColumnId="11"/>
       <queryTableField id="25" name="Attribute Info - Value" tableColumnId="16"/>
-      <queryTableField id="68" dataBound="0" tableColumnId="1"/>
     </queryTableFields>
     <queryTableDeletedFields count="9">
       <deletedField name="Ending 19 Mar"/>
@@ -1023,19 +1097,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55EF3DB-D838-4672-9797-5529200C16EA}" name="Item_Variants34" displayName="Item_Variants34" ref="A1:H224" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:H224" xr:uid="{B1936CF6-5C25-4197-81FE-902107AADDF2}"/>
-  <tableColumns count="8">
-    <tableColumn id="12" xr3:uid="{D49CCDC9-59FE-44C2-BD7D-C3A2541B1643}" uniqueName="12" name="Index" queryTableFieldId="58"/>
-    <tableColumn id="2" xr3:uid="{CBDFBA31-BB2C-4B87-B99D-4FA6484D071B}" uniqueName="2" name="Item Name" queryTableFieldId="2"/>
-    <tableColumn id="5" xr3:uid="{65FFF33C-7188-4522-A8DD-55858C16B4A0}" uniqueName="5" name="Attribute Color - Value" queryTableFieldId="5"/>
-    <tableColumn id="7" xr3:uid="{80D173C5-4704-4349-B0CC-1299BB5D065A}" uniqueName="7" name="Attribute Size - Value" queryTableFieldId="7"/>
-    <tableColumn id="9" xr3:uid="{956CE75D-BB20-4434-ADD5-35F684F60892}" uniqueName="9" name="Attribute Brand - Value" queryTableFieldId="9"/>
-    <tableColumn id="11" xr3:uid="{0AB9E086-7E6E-441C-9985-99F99C361AFE}" uniqueName="11" name="Attribute Season - Value" queryTableFieldId="11"/>
-    <tableColumn id="16" xr3:uid="{D88C1819-3B5A-4CF6-825C-C8BFD3A6ACFA}" uniqueName="16" name="Attribute Info - Value" queryTableFieldId="25"/>
-    <tableColumn id="1" xr3:uid="{5D6217C6-C393-4A8E-8EFE-717BB6469A6F}" uniqueName="1" name="Result" queryTableFieldId="68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C55EF3DB-D838-4672-9797-5529200C16EA}" name="Item_Variants34" displayName="Item_Variants34" ref="A1:G224" tableType="queryTable" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:G224" xr:uid="{B1936CF6-5C25-4197-81FE-902107AADDF2}"/>
+  <tableColumns count="7">
+    <tableColumn id="12" xr3:uid="{D49CCDC9-59FE-44C2-BD7D-C3A2541B1643}" uniqueName="12" name="Index" queryTableFieldId="58" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{CBDFBA31-BB2C-4B87-B99D-4FA6484D071B}" uniqueName="2" name="Item Name" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{65FFF33C-7188-4522-A8DD-55858C16B4A0}" uniqueName="5" name="Attribute Color - Value" queryTableFieldId="5" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{80D173C5-4704-4349-B0CC-1299BB5D065A}" uniqueName="7" name="Attribute Size - Value" queryTableFieldId="7" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{956CE75D-BB20-4434-ADD5-35F684F60892}" uniqueName="9" name="Attribute Brand - Value" queryTableFieldId="9" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{0AB9E086-7E6E-441C-9985-99F99C361AFE}" uniqueName="11" name="Attribute Season - Value" queryTableFieldId="11" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{D88C1819-3B5A-4CF6-825C-C8BFD3A6ACFA}" uniqueName="16" name="Attribute Info - Value" queryTableFieldId="25" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1356,50 +1429,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABEAF2D3-D5CA-4529-BFC2-05E4F94B975D}">
-  <dimension ref="A1:H224"/>
+  <dimension ref="A1:L224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.5546875" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="15.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J1" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1409,14 +1487,20 @@
       <c r="C2" t="s">
         <v>158</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1426,14 +1510,17 @@
       <c r="C3" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1443,14 +1530,14 @@
       <c r="C4" t="s">
         <v>156</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1460,14 +1547,14 @@
       <c r="C5" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1477,14 +1564,14 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1494,31 +1581,31 @@
       <c r="C7" t="s">
         <v>152</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>159</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1528,14 +1615,14 @@
       <c r="C9" t="s">
         <v>158</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1545,14 +1632,14 @@
       <c r="C10" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1562,14 +1649,14 @@
       <c r="C11" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1579,66 +1666,66 @@
       <c r="C12" t="s">
         <v>167</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>166</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>165</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>163</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1649,10 +1736,10 @@
       <c r="B17" t="s">
         <v>162</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
+      <c r="E17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1663,10 +1750,10 @@
       <c r="B18" t="s">
         <v>161</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1677,10 +1764,10 @@
       <c r="B19" t="s">
         <v>160</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
+      <c r="E19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1697,10 +1784,10 @@
       <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G20" t="s">
@@ -1720,10 +1807,10 @@
       <c r="D21" t="s">
         <v>2</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G21" t="s">
@@ -1743,10 +1830,10 @@
       <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
+      <c r="E22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G22" t="s">
@@ -1766,10 +1853,10 @@
       <c r="D23" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1" t="s">
+      <c r="E23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G23" t="s">
@@ -1789,10 +1876,10 @@
       <c r="D24" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G24" t="s">
@@ -1812,10 +1899,10 @@
       <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1" t="s">
+      <c r="E25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G25" t="s">
@@ -1835,10 +1922,10 @@
       <c r="D26" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G26" t="s">
@@ -1858,10 +1945,10 @@
       <c r="D27" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G27" t="s">
@@ -1881,10 +1968,10 @@
       <c r="D28" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G28" t="s">
@@ -1904,10 +1991,10 @@
       <c r="D29" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="E29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G29" t="s">
@@ -1927,10 +2014,10 @@
       <c r="D30" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1" t="s">
+      <c r="E30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G30" t="s">
@@ -1950,10 +2037,10 @@
       <c r="D31" t="s">
         <v>76</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G31" t="s">
@@ -1973,10 +2060,10 @@
       <c r="D32" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="E32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G32" t="s">
@@ -1996,10 +2083,10 @@
       <c r="D33" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1" t="s">
+      <c r="E33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G33" t="s">
@@ -2019,10 +2106,10 @@
       <c r="D34" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G34" t="s">
@@ -2042,10 +2129,10 @@
       <c r="D35" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G35" t="s">
@@ -2065,10 +2152,10 @@
       <c r="D36" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G36" t="s">
@@ -2088,10 +2175,10 @@
       <c r="D37" t="s">
         <v>2</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1" t="s">
+      <c r="E37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G37" t="s">
@@ -2111,10 +2198,10 @@
       <c r="D38" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G38" t="s">
@@ -2134,10 +2221,10 @@
       <c r="D39" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1" t="s">
+      <c r="E39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G39" t="s">
@@ -2157,10 +2244,10 @@
       <c r="D40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F40" s="1" t="s">
+      <c r="E40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G40" t="s">
@@ -2180,10 +2267,10 @@
       <c r="D41" t="s">
         <v>2</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
+      <c r="E41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G41" t="s">
@@ -2203,10 +2290,10 @@
       <c r="D42" t="s">
         <v>2</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G42" t="s">
@@ -2226,10 +2313,10 @@
       <c r="D43" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="1" t="s">
+      <c r="E43" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G43" t="s">
@@ -2249,10 +2336,10 @@
       <c r="D44" t="s">
         <v>78</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G44" t="s">
@@ -2272,10 +2359,10 @@
       <c r="D45" t="s">
         <v>5</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
+      <c r="E45" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G45" t="s">
@@ -2295,10 +2382,10 @@
       <c r="D46" t="s">
         <v>5</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="E46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G46" t="s">
@@ -2318,10 +2405,10 @@
       <c r="D47" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="1" t="s">
+      <c r="E47" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G47" t="s">
@@ -2341,10 +2428,10 @@
       <c r="D48" t="s">
         <v>2</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="1" t="s">
+      <c r="E48" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G48" t="s">
@@ -2364,10 +2451,10 @@
       <c r="D49" t="s">
         <v>2</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F49" s="1" t="s">
+      <c r="E49" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G49" t="s">
@@ -2387,10 +2474,10 @@
       <c r="D50" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F50" s="1" t="s">
+      <c r="E50" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G50" t="s">
@@ -2404,10 +2491,10 @@
       <c r="B51" t="s">
         <v>151</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F51" s="1" t="s">
+      <c r="E51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2421,10 +2508,10 @@
       <c r="C52" t="s">
         <v>12</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F52" s="1" t="s">
+      <c r="E52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2438,10 +2525,10 @@
       <c r="C53" t="s">
         <v>45</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="1" t="s">
+      <c r="E53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2455,10 +2542,10 @@
       <c r="C54" t="s">
         <v>44</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="E54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2472,10 +2559,10 @@
       <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2489,10 +2576,10 @@
       <c r="C56" t="s">
         <v>43</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2506,10 +2593,10 @@
       <c r="C57" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57" s="1" t="s">
+      <c r="E57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2523,10 +2610,10 @@
       <c r="C58" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F58" s="1" t="s">
+      <c r="E58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2540,10 +2627,10 @@
       <c r="C59" t="s">
         <v>41</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F59" s="1" t="s">
+      <c r="E59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2557,10 +2644,10 @@
       <c r="C60" t="s">
         <v>39</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="E60" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2577,10 +2664,10 @@
       <c r="D61" t="s">
         <v>143</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="E61" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2597,10 +2684,10 @@
       <c r="D62" t="s">
         <v>145</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="E62" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2617,10 +2704,10 @@
       <c r="D63" t="s">
         <v>143</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="E63" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2637,10 +2724,10 @@
       <c r="D64" t="s">
         <v>146</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="E64" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2657,10 +2744,10 @@
       <c r="D65" t="s">
         <v>145</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F65" s="1" t="s">
+      <c r="E65" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2677,10 +2764,10 @@
       <c r="D66" t="s">
         <v>145</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="E66" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2697,10 +2784,10 @@
       <c r="D67" t="s">
         <v>143</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F67" s="1" t="s">
+      <c r="E67" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2717,10 +2804,10 @@
       <c r="D68" t="s">
         <v>147</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F68" s="1" t="s">
+      <c r="E68" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2737,10 +2824,10 @@
       <c r="D69" t="s">
         <v>146</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F69" s="1" t="s">
+      <c r="E69" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2757,10 +2844,10 @@
       <c r="D70" t="s">
         <v>145</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F70" s="1" t="s">
+      <c r="E70" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2777,10 +2864,10 @@
       <c r="D71" t="s">
         <v>143</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F71" s="1" t="s">
+      <c r="E71" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2797,10 +2884,10 @@
       <c r="D72" t="s">
         <v>145</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F72" s="1" t="s">
+      <c r="E72" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2817,10 +2904,10 @@
       <c r="D73" t="s">
         <v>143</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F73" s="1" t="s">
+      <c r="E73" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2837,10 +2924,10 @@
       <c r="D74" t="s">
         <v>141</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F74" s="1" t="s">
+      <c r="E74" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2857,10 +2944,10 @@
       <c r="D75" t="s">
         <v>119</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F75" s="1" t="s">
+      <c r="E75" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2877,10 +2964,10 @@
       <c r="D76" t="s">
         <v>123</v>
       </c>
-      <c r="E76" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F76" s="1" t="s">
+      <c r="E76" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2897,10 +2984,10 @@
       <c r="D77" t="s">
         <v>141</v>
       </c>
-      <c r="E77" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F77" s="1" t="s">
+      <c r="E77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2917,10 +3004,10 @@
       <c r="D78" t="s">
         <v>119</v>
       </c>
-      <c r="E78" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F78" s="1" t="s">
+      <c r="E78" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F78" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2937,10 +3024,10 @@
       <c r="D79" t="s">
         <v>141</v>
       </c>
-      <c r="E79" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F79" s="1" t="s">
+      <c r="E79" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2957,10 +3044,10 @@
       <c r="D80" t="s">
         <v>119</v>
       </c>
-      <c r="E80" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F80" s="1" t="s">
+      <c r="E80" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2977,10 +3064,10 @@
       <c r="D81" t="s">
         <v>141</v>
       </c>
-      <c r="E81" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F81" s="1" t="s">
+      <c r="E81" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F81" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2997,10 +3084,10 @@
       <c r="D82" t="s">
         <v>119</v>
       </c>
-      <c r="E82" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F82" s="1" t="s">
+      <c r="E82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F82" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3017,10 +3104,10 @@
       <c r="D83" t="s">
         <v>115</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1" t="s">
+      <c r="E83" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3037,10 +3124,10 @@
       <c r="D84" t="s">
         <v>115</v>
       </c>
-      <c r="E84" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1" t="s">
+      <c r="E84" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F84" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3057,10 +3144,10 @@
       <c r="D85" t="s">
         <v>108</v>
       </c>
-      <c r="E85" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F85" s="1" t="s">
+      <c r="E85" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3077,10 +3164,10 @@
       <c r="D86" t="s">
         <v>141</v>
       </c>
-      <c r="E86" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F86" s="1" t="s">
+      <c r="E86" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3097,10 +3184,10 @@
       <c r="D87" t="s">
         <v>123</v>
       </c>
-      <c r="E87" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F87" s="1" t="s">
+      <c r="E87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3117,10 +3204,10 @@
       <c r="D88" t="s">
         <v>108</v>
       </c>
-      <c r="E88" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F88" s="1" t="s">
+      <c r="E88" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3137,10 +3224,10 @@
       <c r="D89" t="s">
         <v>115</v>
       </c>
-      <c r="E89" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F89" s="1" t="s">
+      <c r="E89" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3157,10 +3244,10 @@
       <c r="D90" t="s">
         <v>115</v>
       </c>
-      <c r="E90" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F90" s="1" t="s">
+      <c r="E90" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3177,10 +3264,10 @@
       <c r="D91" t="s">
         <v>134</v>
       </c>
-      <c r="E91" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F91" s="1" t="s">
+      <c r="E91" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3197,10 +3284,10 @@
       <c r="D92" t="s">
         <v>124</v>
       </c>
-      <c r="E92" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F92" s="1" t="s">
+      <c r="E92" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3217,10 +3304,10 @@
       <c r="D93" t="s">
         <v>131</v>
       </c>
-      <c r="E93" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F93" s="1" t="s">
+      <c r="E93" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3237,10 +3324,10 @@
       <c r="D94" t="s">
         <v>133</v>
       </c>
-      <c r="E94" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F94" s="1" t="s">
+      <c r="E94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F94" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3257,10 +3344,10 @@
       <c r="D95" t="s">
         <v>126</v>
       </c>
-      <c r="E95" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F95" s="1" t="s">
+      <c r="E95" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3277,10 +3364,10 @@
       <c r="D96" t="s">
         <v>136</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F96" s="1" t="s">
+      <c r="E96" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3297,10 +3384,10 @@
       <c r="D97" t="s">
         <v>134</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F97" s="1" t="s">
+      <c r="E97" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F97" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3317,10 +3404,10 @@
       <c r="D98" t="s">
         <v>133</v>
       </c>
-      <c r="E98" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F98" s="1" t="s">
+      <c r="E98" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3337,10 +3424,10 @@
       <c r="D99" t="s">
         <v>126</v>
       </c>
-      <c r="E99" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F99" s="1" t="s">
+      <c r="E99" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3357,10 +3444,10 @@
       <c r="D100" t="s">
         <v>130</v>
       </c>
-      <c r="E100" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F100" s="1" t="s">
+      <c r="E100" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3377,10 +3464,10 @@
       <c r="D101" t="s">
         <v>132</v>
       </c>
-      <c r="E101" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F101" s="1" t="s">
+      <c r="E101" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F101" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3397,10 +3484,10 @@
       <c r="D102" t="s">
         <v>131</v>
       </c>
-      <c r="E102" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F102" s="1" t="s">
+      <c r="E102" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3417,10 +3504,10 @@
       <c r="D103" t="s">
         <v>130</v>
       </c>
-      <c r="E103" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F103" s="1" t="s">
+      <c r="E103" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F103" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3437,10 +3524,10 @@
       <c r="D104" t="s">
         <v>128</v>
       </c>
-      <c r="E104" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F104" s="1" t="s">
+      <c r="E104" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3457,10 +3544,10 @@
       <c r="D105" t="s">
         <v>126</v>
       </c>
-      <c r="E105" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F105" s="1" t="s">
+      <c r="E105" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F105" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3477,10 +3564,10 @@
       <c r="D106" t="s">
         <v>124</v>
       </c>
-      <c r="E106" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F106" s="1" t="s">
+      <c r="E106" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F106" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3497,10 +3584,10 @@
       <c r="D107" t="s">
         <v>119</v>
       </c>
-      <c r="E107" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F107" s="1" t="s">
+      <c r="E107" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3517,10 +3604,10 @@
       <c r="D108" t="s">
         <v>123</v>
       </c>
-      <c r="E108" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F108" s="1" t="s">
+      <c r="E108" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F108" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3537,10 +3624,10 @@
       <c r="D109" t="s">
         <v>115</v>
       </c>
-      <c r="E109" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F109" s="1" t="s">
+      <c r="E109" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F109" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3557,10 +3644,10 @@
       <c r="D110" t="s">
         <v>108</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F110" s="1" t="s">
+      <c r="E110" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3577,10 +3664,10 @@
       <c r="D111" t="s">
         <v>119</v>
       </c>
-      <c r="E111" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F111" s="1" t="s">
+      <c r="E111" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F111" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3597,10 +3684,10 @@
       <c r="D112" t="s">
         <v>119</v>
       </c>
-      <c r="E112" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F112" s="1" t="s">
+      <c r="E112" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3617,10 +3704,10 @@
       <c r="D113" t="s">
         <v>119</v>
       </c>
-      <c r="E113" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F113" s="1" t="s">
+      <c r="E113" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F113" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3637,10 +3724,10 @@
       <c r="D114" t="s">
         <v>108</v>
       </c>
-      <c r="E114" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F114" s="1" t="s">
+      <c r="E114" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F114" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3657,10 +3744,10 @@
       <c r="D115" t="s">
         <v>115</v>
       </c>
-      <c r="E115" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F115" s="1" t="s">
+      <c r="E115" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F115" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3677,10 +3764,10 @@
       <c r="D116" t="s">
         <v>111</v>
       </c>
-      <c r="E116" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F116" s="1" t="s">
+      <c r="E116" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F116" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3697,10 +3784,10 @@
       <c r="D117" t="s">
         <v>111</v>
       </c>
-      <c r="E117" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F117" s="1" t="s">
+      <c r="E117" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F117" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3717,10 +3804,10 @@
       <c r="D118" t="s">
         <v>108</v>
       </c>
-      <c r="E118" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F118" s="1" t="s">
+      <c r="E118" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F118" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3734,10 +3821,10 @@
       <c r="C119" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F119" s="1" t="s">
+      <c r="E119" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F119" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3754,10 +3841,10 @@
       <c r="D120" t="s">
         <v>14</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F120" s="1" t="s">
+      <c r="E120" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F120" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3774,10 +3861,10 @@
       <c r="D121" t="s">
         <v>14</v>
       </c>
-      <c r="E121" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F121" s="1" t="s">
+      <c r="E121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F121" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3794,10 +3881,10 @@
       <c r="D122" t="s">
         <v>24</v>
       </c>
-      <c r="E122" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F122" s="1" t="s">
+      <c r="E122" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F122" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3814,10 +3901,10 @@
       <c r="D123" t="s">
         <v>24</v>
       </c>
-      <c r="E123" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F123" s="1" t="s">
+      <c r="E123" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F123" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3834,10 +3921,10 @@
       <c r="D124" t="s">
         <v>24</v>
       </c>
-      <c r="E124" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F124" s="1" t="s">
+      <c r="E124" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F124" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3854,10 +3941,10 @@
       <c r="D125" t="s">
         <v>24</v>
       </c>
-      <c r="E125" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F125" s="1" t="s">
+      <c r="E125" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F125" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3871,10 +3958,10 @@
       <c r="C126" t="s">
         <v>44</v>
       </c>
-      <c r="E126" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F126" s="1" t="s">
+      <c r="E126" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F126" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3888,10 +3975,10 @@
       <c r="C127" t="s">
         <v>12</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F127" s="1" t="s">
+      <c r="E127" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F127" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3905,10 +3992,10 @@
       <c r="C128" t="s">
         <v>43</v>
       </c>
-      <c r="E128" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F128" s="1" t="s">
+      <c r="E128" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F128" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3922,10 +4009,10 @@
       <c r="C129" t="s">
         <v>8</v>
       </c>
-      <c r="E129" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F129" s="1" t="s">
+      <c r="E129" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F129" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3936,10 +4023,10 @@
       <c r="B130" t="s">
         <v>101</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F130" s="1" t="s">
+      <c r="E130" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F130" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G130" t="s">
@@ -3953,10 +4040,10 @@
       <c r="B131" t="s">
         <v>101</v>
       </c>
-      <c r="E131" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F131" s="1" t="s">
+      <c r="E131" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F131" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G131" t="s">
@@ -3970,10 +4057,10 @@
       <c r="B132" t="s">
         <v>101</v>
       </c>
-      <c r="E132" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F132" s="1" t="s">
+      <c r="E132" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F132" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G132" t="s">
@@ -3987,10 +4074,10 @@
       <c r="B133" t="s">
         <v>95</v>
       </c>
-      <c r="E133" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F133" s="1" t="s">
+      <c r="E133" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F133" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G133" t="s">
@@ -4004,10 +4091,10 @@
       <c r="B134" t="s">
         <v>95</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F134" s="1" t="s">
+      <c r="E134" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F134" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G134" t="s">
@@ -4021,10 +4108,10 @@
       <c r="B135" t="s">
         <v>95</v>
       </c>
-      <c r="E135" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F135" s="1" t="s">
+      <c r="E135" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F135" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G135" t="s">
@@ -4038,10 +4125,10 @@
       <c r="B136" t="s">
         <v>95</v>
       </c>
-      <c r="E136" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F136" s="1" t="s">
+      <c r="E136" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F136" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G136" t="s">
@@ -4055,10 +4142,10 @@
       <c r="B137" t="s">
         <v>95</v>
       </c>
-      <c r="E137" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F137" s="1" t="s">
+      <c r="E137" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F137" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G137" t="s">
@@ -4072,10 +4159,10 @@
       <c r="B138" t="s">
         <v>90</v>
       </c>
-      <c r="E138" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F138" s="1" t="s">
+      <c r="E138" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F138" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G138" t="s">
@@ -4089,10 +4176,10 @@
       <c r="B139" t="s">
         <v>90</v>
       </c>
-      <c r="E139" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F139" s="1" t="s">
+      <c r="E139" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F139" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G139" t="s">
@@ -4106,10 +4193,10 @@
       <c r="B140" t="s">
         <v>90</v>
       </c>
-      <c r="E140" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F140" s="1" t="s">
+      <c r="E140" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F140" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G140" t="s">
@@ -4123,10 +4210,10 @@
       <c r="B141" t="s">
         <v>90</v>
       </c>
-      <c r="E141" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F141" s="1" t="s">
+      <c r="E141" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F141" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G141" t="s">
@@ -4140,10 +4227,10 @@
       <c r="B142" t="s">
         <v>87</v>
       </c>
-      <c r="E142" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F142" s="1" t="s">
+      <c r="E142" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F142" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G142" t="s">
@@ -4157,10 +4244,10 @@
       <c r="B143" t="s">
         <v>87</v>
       </c>
-      <c r="E143" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F143" s="1" t="s">
+      <c r="E143" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F143" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G143" t="s">
@@ -4174,10 +4261,10 @@
       <c r="B144" t="s">
         <v>83</v>
       </c>
-      <c r="E144" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F144" s="1" t="s">
+      <c r="E144" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F144" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G144" t="s">
@@ -4191,10 +4278,10 @@
       <c r="B145" t="s">
         <v>83</v>
       </c>
-      <c r="E145" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F145" s="1" t="s">
+      <c r="E145" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F145" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G145" t="s">
@@ -4208,10 +4295,10 @@
       <c r="B146" t="s">
         <v>83</v>
       </c>
-      <c r="E146" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F146" s="1" t="s">
+      <c r="E146" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F146" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G146" t="s">
@@ -4228,10 +4315,10 @@
       <c r="D147" t="s">
         <v>5</v>
       </c>
-      <c r="E147" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F147" s="1" t="s">
+      <c r="E147" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F147" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4245,10 +4332,10 @@
       <c r="D148" t="s">
         <v>2</v>
       </c>
-      <c r="E148" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F148" s="1" t="s">
+      <c r="E148" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F148" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4262,10 +4349,10 @@
       <c r="D149" t="s">
         <v>76</v>
       </c>
-      <c r="E149" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F149" s="1" t="s">
+      <c r="E149" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F149" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4279,10 +4366,10 @@
       <c r="D150" t="s">
         <v>78</v>
       </c>
-      <c r="E150" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F150" s="1" t="s">
+      <c r="E150" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F150" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4296,10 +4383,10 @@
       <c r="D151" t="s">
         <v>5</v>
       </c>
-      <c r="E151" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F151" s="1" t="s">
+      <c r="E151" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4313,10 +4400,10 @@
       <c r="D152" t="s">
         <v>2</v>
       </c>
-      <c r="E152" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F152" s="1" t="s">
+      <c r="E152" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F152" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4330,10 +4417,10 @@
       <c r="D153" t="s">
         <v>77</v>
       </c>
-      <c r="E153" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F153" s="1" t="s">
+      <c r="E153" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F153" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4347,10 +4434,10 @@
       <c r="D154" t="s">
         <v>76</v>
       </c>
-      <c r="E154" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F154" s="1" t="s">
+      <c r="E154" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F154" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4364,10 +4451,10 @@
       <c r="D155" t="s">
         <v>74</v>
       </c>
-      <c r="E155" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F155" s="1" t="s">
+      <c r="E155" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F155" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4381,10 +4468,10 @@
       <c r="D156" t="s">
         <v>78</v>
       </c>
-      <c r="E156" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F156" s="1" t="s">
+      <c r="E156" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F156" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4398,10 +4485,10 @@
       <c r="D157" t="s">
         <v>5</v>
       </c>
-      <c r="E157" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F157" s="1" t="s">
+      <c r="E157" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F157" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4415,10 +4502,10 @@
       <c r="D158" t="s">
         <v>2</v>
       </c>
-      <c r="E158" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F158" s="1" t="s">
+      <c r="E158" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F158" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4432,10 +4519,10 @@
       <c r="D159" t="s">
         <v>77</v>
       </c>
-      <c r="E159" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F159" s="1" t="s">
+      <c r="E159" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F159" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4449,10 +4536,10 @@
       <c r="D160" t="s">
         <v>76</v>
       </c>
-      <c r="E160" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F160" s="1" t="s">
+      <c r="E160" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F160" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4466,10 +4553,10 @@
       <c r="D161" t="s">
         <v>74</v>
       </c>
-      <c r="E161" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F161" s="1" t="s">
+      <c r="E161" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F161" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4483,10 +4570,10 @@
       <c r="D162" t="s">
         <v>72</v>
       </c>
-      <c r="E162" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F162" s="1" t="s">
+      <c r="E162" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F162" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4500,10 +4587,10 @@
       <c r="D163" t="s">
         <v>70</v>
       </c>
-      <c r="E163" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F163" s="1" t="s">
+      <c r="E163" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F163" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4514,10 +4601,10 @@
       <c r="B164" t="s">
         <v>69</v>
       </c>
-      <c r="E164" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F164" s="1" t="s">
+      <c r="E164" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F164" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4528,10 +4615,10 @@
       <c r="B165" t="s">
         <v>68</v>
       </c>
-      <c r="E165" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F165" s="1" t="s">
+      <c r="E165" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4542,10 +4629,10 @@
       <c r="B166" t="s">
         <v>67</v>
       </c>
-      <c r="E166" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F166" s="1" t="s">
+      <c r="E166" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F166" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4556,10 +4643,10 @@
       <c r="B167" t="s">
         <v>50</v>
       </c>
-      <c r="E167" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F167" s="1" t="s">
+      <c r="E167" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F167" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G167" t="s">
@@ -4573,10 +4660,10 @@
       <c r="B168" t="s">
         <v>50</v>
       </c>
-      <c r="E168" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F168" s="1" t="s">
+      <c r="E168" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F168" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G168" t="s">
@@ -4590,10 +4677,10 @@
       <c r="B169" t="s">
         <v>50</v>
       </c>
-      <c r="E169" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F169" s="1" t="s">
+      <c r="E169" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F169" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G169" t="s">
@@ -4607,10 +4694,10 @@
       <c r="B170" t="s">
         <v>50</v>
       </c>
-      <c r="E170" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F170" s="1" t="s">
+      <c r="E170" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F170" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G170" t="s">
@@ -4624,10 +4711,10 @@
       <c r="B171" t="s">
         <v>50</v>
       </c>
-      <c r="E171" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F171" s="1" t="s">
+      <c r="E171" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F171" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G171" t="s">
@@ -4641,10 +4728,10 @@
       <c r="B172" t="s">
         <v>50</v>
       </c>
-      <c r="E172" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F172" s="1" t="s">
+      <c r="E172" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F172" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G172" t="s">
@@ -4658,10 +4745,10 @@
       <c r="B173" t="s">
         <v>50</v>
       </c>
-      <c r="E173" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F173" s="1" t="s">
+      <c r="E173" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F173" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G173" t="s">
@@ -4675,10 +4762,10 @@
       <c r="B174" t="s">
         <v>50</v>
       </c>
-      <c r="E174" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F174" s="1" t="s">
+      <c r="E174" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F174" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G174" t="s">
@@ -4692,10 +4779,10 @@
       <c r="B175" t="s">
         <v>50</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F175" s="1" t="s">
+      <c r="E175" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F175" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G175" t="s">
@@ -4709,10 +4796,10 @@
       <c r="B176" t="s">
         <v>50</v>
       </c>
-      <c r="E176" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F176" s="1" t="s">
+      <c r="E176" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F176" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G176" t="s">
@@ -4726,10 +4813,10 @@
       <c r="B177" t="s">
         <v>50</v>
       </c>
-      <c r="E177" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F177" s="1" t="s">
+      <c r="E177" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F177" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G177" t="s">
@@ -4743,10 +4830,10 @@
       <c r="B178" t="s">
         <v>50</v>
       </c>
-      <c r="E178" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F178" s="1" t="s">
+      <c r="E178" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F178" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G178" t="s">
@@ -4760,10 +4847,10 @@
       <c r="B179" t="s">
         <v>50</v>
       </c>
-      <c r="E179" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F179" s="1" t="s">
+      <c r="E179" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F179" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G179" t="s">
@@ -4777,10 +4864,10 @@
       <c r="B180" t="s">
         <v>50</v>
       </c>
-      <c r="E180" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F180" s="1" t="s">
+      <c r="E180" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F180" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G180" t="s">
@@ -4794,10 +4881,10 @@
       <c r="B181" t="s">
         <v>50</v>
       </c>
-      <c r="E181" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F181" s="1" t="s">
+      <c r="E181" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F181" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G181" t="s">
@@ -4811,10 +4898,10 @@
       <c r="B182" t="s">
         <v>50</v>
       </c>
-      <c r="E182" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F182" s="1" t="s">
+      <c r="E182" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F182" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G182" t="s">
@@ -4828,10 +4915,10 @@
       <c r="B183" t="s">
         <v>50</v>
       </c>
-      <c r="E183" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F183" s="1" t="s">
+      <c r="E183" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F183" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G183" t="s">
@@ -4851,10 +4938,10 @@
       <c r="D184" t="s">
         <v>48</v>
       </c>
-      <c r="E184" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F184" s="1" t="s">
+      <c r="E184" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F184" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4871,10 +4958,10 @@
       <c r="D185" t="s">
         <v>46</v>
       </c>
-      <c r="E185" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F185" s="1" t="s">
+      <c r="E185" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F185" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4888,10 +4975,10 @@
       <c r="C186" t="s">
         <v>45</v>
       </c>
-      <c r="E186" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F186" s="1" t="s">
+      <c r="E186" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F186" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4905,10 +4992,10 @@
       <c r="C187" t="s">
         <v>44</v>
       </c>
-      <c r="E187" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F187" s="1" t="s">
+      <c r="E187" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F187" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4922,10 +5009,10 @@
       <c r="C188" t="s">
         <v>12</v>
       </c>
-      <c r="E188" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F188" s="1" t="s">
+      <c r="E188" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F188" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4939,10 +5026,10 @@
       <c r="C189" t="s">
         <v>43</v>
       </c>
-      <c r="E189" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F189" s="1" t="s">
+      <c r="E189" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F189" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4956,10 +5043,10 @@
       <c r="C190" t="s">
         <v>42</v>
       </c>
-      <c r="E190" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F190" s="1" t="s">
+      <c r="E190" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F190" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4973,10 +5060,10 @@
       <c r="C191" t="s">
         <v>8</v>
       </c>
-      <c r="E191" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F191" s="1" t="s">
+      <c r="E191" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F191" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4990,10 +5077,10 @@
       <c r="C192" t="s">
         <v>41</v>
       </c>
-      <c r="E192" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F192" s="1" t="s">
+      <c r="E192" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F192" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5007,10 +5094,10 @@
       <c r="C193" t="s">
         <v>39</v>
       </c>
-      <c r="E193" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F193" s="1" t="s">
+      <c r="E193" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F193" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5021,10 +5108,10 @@
       <c r="B194" t="s">
         <v>38</v>
       </c>
-      <c r="E194" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F194" s="1" t="s">
+      <c r="E194" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F194" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5038,10 +5125,10 @@
       <c r="C195" t="s">
         <v>35</v>
       </c>
-      <c r="E195" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F195" s="1" t="s">
+      <c r="E195" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F195" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5055,10 +5142,10 @@
       <c r="C196" t="s">
         <v>35</v>
       </c>
-      <c r="E196" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F196" s="1" t="s">
+      <c r="E196" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F196" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5075,10 +5162,10 @@
       <c r="D197" t="s">
         <v>7</v>
       </c>
-      <c r="E197" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F197" s="1" t="s">
+      <c r="E197" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F197" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5095,10 +5182,10 @@
       <c r="D198" t="s">
         <v>28</v>
       </c>
-      <c r="E198" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F198" s="1" t="s">
+      <c r="E198" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F198" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5115,10 +5202,10 @@
       <c r="D199" t="s">
         <v>28</v>
       </c>
-      <c r="E199" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F199" s="1" t="s">
+      <c r="E199" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F199" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5135,10 +5222,10 @@
       <c r="D200" t="s">
         <v>28</v>
       </c>
-      <c r="E200" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F200" s="1" t="s">
+      <c r="E200" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F200" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5155,10 +5242,10 @@
       <c r="D201" t="s">
         <v>28</v>
       </c>
-      <c r="E201" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F201" s="1" t="s">
+      <c r="E201" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F201" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5172,10 +5259,10 @@
       <c r="C202" t="s">
         <v>13</v>
       </c>
-      <c r="E202" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F202" s="1" t="s">
+      <c r="E202" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F202" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5189,10 +5276,10 @@
       <c r="C203" t="s">
         <v>12</v>
       </c>
-      <c r="E203" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F203" s="1" t="s">
+      <c r="E203" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F203" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5206,10 +5293,10 @@
       <c r="C204" t="s">
         <v>10</v>
       </c>
-      <c r="E204" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F204" s="1" t="s">
+      <c r="E204" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F204" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5226,10 +5313,10 @@
       <c r="D205" t="s">
         <v>24</v>
       </c>
-      <c r="E205" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F205" s="1" t="s">
+      <c r="E205" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F205" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5246,10 +5333,10 @@
       <c r="D206" t="s">
         <v>18</v>
       </c>
-      <c r="E206" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F206" s="1" t="s">
+      <c r="E206" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F206" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5266,10 +5353,10 @@
       <c r="D207" t="s">
         <v>18</v>
       </c>
-      <c r="E207" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F207" s="1" t="s">
+      <c r="E207" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F207" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5286,10 +5373,10 @@
       <c r="D208" t="s">
         <v>18</v>
       </c>
-      <c r="E208" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F208" s="1" t="s">
+      <c r="E208" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F208" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5306,10 +5393,10 @@
       <c r="D209" t="s">
         <v>18</v>
       </c>
-      <c r="E209" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F209" s="1" t="s">
+      <c r="E209" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F209" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5326,10 +5413,10 @@
       <c r="D210" t="s">
         <v>24</v>
       </c>
-      <c r="E210" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F210" s="1" t="s">
+      <c r="E210" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F210" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5346,10 +5433,10 @@
       <c r="D211" t="s">
         <v>18</v>
       </c>
-      <c r="E211" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F211" s="1" t="s">
+      <c r="E211" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F211" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5366,10 +5453,10 @@
       <c r="D212" t="s">
         <v>18</v>
       </c>
-      <c r="E212" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F212" s="1" t="s">
+      <c r="E212" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F212" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5386,10 +5473,10 @@
       <c r="D213" t="s">
         <v>18</v>
       </c>
-      <c r="E213" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F213" s="1" t="s">
+      <c r="E213" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F213" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5406,10 +5493,10 @@
       <c r="D214" t="s">
         <v>18</v>
       </c>
-      <c r="E214" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F214" s="1" t="s">
+      <c r="E214" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F214" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5426,10 +5513,10 @@
       <c r="D215" t="s">
         <v>14</v>
       </c>
-      <c r="E215" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F215" s="1" t="s">
+      <c r="E215" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F215" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5446,10 +5533,10 @@
       <c r="D216" t="s">
         <v>17</v>
       </c>
-      <c r="E216" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F216" s="1" t="s">
+      <c r="E216" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F216" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5466,10 +5553,10 @@
       <c r="D217" t="s">
         <v>14</v>
       </c>
-      <c r="E217" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F217" s="1" t="s">
+      <c r="E217" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F217" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5486,10 +5573,10 @@
       <c r="D218" t="s">
         <v>7</v>
       </c>
-      <c r="E218" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F218" s="1" t="s">
+      <c r="E218" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F218" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5506,10 +5593,10 @@
       <c r="D219" t="s">
         <v>7</v>
       </c>
-      <c r="E219" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F219" s="1" t="s">
+      <c r="E219" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F219" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5526,10 +5613,10 @@
       <c r="D220" t="s">
         <v>11</v>
       </c>
-      <c r="E220" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F220" s="1" t="s">
+      <c r="E220" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F220" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5546,10 +5633,10 @@
       <c r="D221" t="s">
         <v>7</v>
       </c>
-      <c r="E221" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F221" s="1" t="s">
+      <c r="E221" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F221" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5566,10 +5653,10 @@
       <c r="D222" t="s">
         <v>7</v>
       </c>
-      <c r="E222" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F222" s="1" t="s">
+      <c r="E222" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F222" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5586,10 +5673,10 @@
       <c r="D223" t="s">
         <v>5</v>
       </c>
-      <c r="E223" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F223" s="1" t="s">
+      <c r="E223" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F223" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5606,10 +5693,10 @@
       <c r="D224" t="s">
         <v>2</v>
       </c>
-      <c r="E224" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F224" s="1" t="s">
+      <c r="E224" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F224" s="3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>